<commit_message>
feat : Add PrefabsToCSVSaver
</commit_message>
<xml_diff>
--- a/Assets/KSI/Data/Item.xlsx
+++ b/Assets/KSI/Data/Item.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KANGSOOIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KANGSOOIN\Desktop\LLuckyStudio\Assets\KSI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3193A8C-F358-487C-B040-EA6D7F324AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC31E2-C087-481E-846F-9600894EE2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="735" windowWidth="14400" windowHeight="15360" xr2:uid="{686E87A2-2C89-4B63-8C24-344EC070C321}"/>
+    <workbookView xWindow="12705" yWindow="1830" windowWidth="14400" windowHeight="8850" xr2:uid="{686E87A2-2C89-4B63-8C24-344EC070C321}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>